<commit_message>
add comments into our sample workbook
</commit_message>
<xml_diff>
--- a/src/openapi2excel.tests/Sample/sample-api-gw.xlsx
+++ b/src/openapi2excel.tests/Sample/sample-api-gw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\darrenwest-allocate\openapi-2-excel\src\openapi2excel.tests\Sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3733D738-3860-4624-8A34-3C245940E06E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2575843E-1280-4443-B090-78DE0B7DCC1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,145 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={D18CFDBA-147F-42A3-B5C8-D5413335E96B}</author>
+  </authors>
+  <commentList>
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{D18CFDBA-147F-42A3-B5C8-D5413335E96B}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A comment from the summary page about a endpoint link</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={8F812A0B-C25E-4558-B067-101CA992F2D2}</author>
+    <author>tc={38372118-311B-4E12-9E8D-1103BB168BE2}</author>
+    <author>tc={75DB1C0F-DDE3-4804-9FF1-C04CE0245A16}</author>
+  </authors>
+  <commentList>
+    <comment ref="D6" authorId="0" shapeId="0" xr:uid="{8F812A0B-C25E-4558-B067-101CA992F2D2}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A comment about a description
+Reply:
+    A threaded reply where there is more infomation</t>
+      </text>
+    </comment>
+    <comment ref="A12" authorId="1" shapeId="0" xr:uid="{38372118-311B-4E12-9E8D-1103BB168BE2}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A comment that we will marked resolved</t>
+      </text>
+    </comment>
+    <comment ref="M25" authorId="2" shapeId="0" xr:uid="{75DB1C0F-DDE3-4804-9FF1-C04CE0245A16}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A comment in a field that was not populated by the open api json</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={7390FAAB-D469-484C-8448-07C57D04C27F}</author>
+    <author>tc={4998275B-65B9-4E36-AD9C-B19044100824}</author>
+  </authors>
+  <commentList>
+    <comment ref="Q30" authorId="0" shapeId="0" xr:uid="{7390FAAB-D469-484C-8448-07C57D04C27F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A comment on the next tab 02
+Reply:
+    Threaded dicussion where we mention @Darren.West</t>
+      </text>
+    </comment>
+    <comment ref="E31" authorId="1" shapeId="0" xr:uid="{4998275B-65B9-4E36-AD9C-B19044100824}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A comment on the next tab 01</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={BE93D9E9-6A4E-4E47-9AC0-D71186EB2766}</author>
+    <author>tc={B6CA6A55-4FE8-46C2-900B-A836F1375FBF}</author>
+    <author>tc={2C0C78C8-DC0E-4139-9F5F-464B2DA390A9}</author>
+  </authors>
+  <commentList>
+    <comment ref="M5" authorId="0" shapeId="0" xr:uid="{BE93D9E9-6A4E-4E47-9AC0-D71186EB2766}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A random comment somewhere on the page</t>
+      </text>
+    </comment>
+    <comment ref="A30" authorId="1" shapeId="0" xr:uid="{B6CA6A55-4FE8-46C2-900B-A836F1375FBF}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A comment about the response options</t>
+      </text>
+    </comment>
+    <comment ref="A31" authorId="2" shapeId="0" xr:uid="{2C0C78C8-DC0E-4139-9F5F-464B2DA390A9}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Another response that gets another comment</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={E39844C5-218E-4325-9139-8E3E6C8F9199}</author>
+  </authors>
+  <commentList>
+    <comment ref="C28" authorId="0" shapeId="0" xr:uid="{E39844C5-218E-4325-9139-8E3E6C8F9199}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This comment is for a column that is missing any values</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="107">
   <si>
@@ -353,7 +492,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -386,6 +525,12 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -450,6 +595,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Darren West" id="{0E5F8CFF-5CBB-4BE3-A17F-527DE6B9C210}" userId="S::darren.west@rldatix.com::7391f33d-5233-4345-9e24-9321d78f6ab7" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -735,11 +886,74 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B3" dT="2025-09-21T17:44:49.44" personId="{0E5F8CFF-5CBB-4BE3-A17F-527DE6B9C210}" id="{D18CFDBA-147F-42A3-B5C8-D5413335E96B}">
+    <text>A comment from the summary page about a endpoint link</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="D6" dT="2025-09-21T17:45:02.30" personId="{0E5F8CFF-5CBB-4BE3-A17F-527DE6B9C210}" id="{8F812A0B-C25E-4558-B067-101CA992F2D2}">
+    <text>A comment about a description</text>
+  </threadedComment>
+  <threadedComment ref="D6" dT="2025-09-21T17:45:13.83" personId="{0E5F8CFF-5CBB-4BE3-A17F-527DE6B9C210}" id="{006CFE16-D608-4ED5-9EA8-037DEA364F8A}" parentId="{8F812A0B-C25E-4558-B067-101CA992F2D2}">
+    <text>A threaded reply where there is more infomation</text>
+  </threadedComment>
+  <threadedComment ref="A12" dT="2025-09-21T17:46:03.58" personId="{0E5F8CFF-5CBB-4BE3-A17F-527DE6B9C210}" id="{38372118-311B-4E12-9E8D-1103BB168BE2}" done="1">
+    <text>A comment that we will marked resolved</text>
+  </threadedComment>
+  <threadedComment ref="M25" dT="2025-09-21T17:46:46.98" personId="{0E5F8CFF-5CBB-4BE3-A17F-527DE6B9C210}" id="{75DB1C0F-DDE3-4804-9FF1-C04CE0245A16}">
+    <text>A comment in a field that was not populated by the open api json</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment3.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="Q30" dT="2025-09-21T17:47:16.42" personId="{0E5F8CFF-5CBB-4BE3-A17F-527DE6B9C210}" id="{7390FAAB-D469-484C-8448-07C57D04C27F}">
+    <text>A comment on the next tab 02</text>
+  </threadedComment>
+  <threadedComment ref="Q30" dT="2025-09-21T17:47:37.38" personId="{0E5F8CFF-5CBB-4BE3-A17F-527DE6B9C210}" id="{A61D7B80-5C20-4265-A09D-E92ACDB827E1}" parentId="{7390FAAB-D469-484C-8448-07C57D04C27F}">
+    <text>Threaded dicussion where we mention @Darren.West</text>
+  </threadedComment>
+  <threadedComment ref="E31" dT="2025-09-21T17:47:07.12" personId="{0E5F8CFF-5CBB-4BE3-A17F-527DE6B9C210}" id="{4998275B-65B9-4E36-AD9C-B19044100824}">
+    <text>A comment on the next tab 01</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment4.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="M5" dT="2025-09-21T17:48:14.98" personId="{0E5F8CFF-5CBB-4BE3-A17F-527DE6B9C210}" id="{BE93D9E9-6A4E-4E47-9AC0-D71186EB2766}">
+    <text>A random comment somewhere on the page</text>
+  </threadedComment>
+  <threadedComment ref="A30" dT="2025-09-21T17:48:01.24" personId="{0E5F8CFF-5CBB-4BE3-A17F-527DE6B9C210}" id="{B6CA6A55-4FE8-46C2-900B-A836F1375FBF}">
+    <text>A comment about the response options</text>
+  </threadedComment>
+  <threadedComment ref="A31" dT="2025-09-21T17:48:38.25" personId="{0E5F8CFF-5CBB-4BE3-A17F-527DE6B9C210}" id="{2C0C78C8-DC0E-4139-9F5F-464B2DA390A9}">
+    <text>Another response that gets another comment</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment5.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="C28" dT="2025-09-21T17:49:04.52" personId="{0E5F8CFF-5CBB-4BE3-A17F-527DE6B9C210}" id="{E39844C5-218E-4325-9139-8E3E6C8F9199}">
+    <text>This comment is for a column that is missing any values</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -826,17 +1040,20 @@
     <hyperlink ref="B8" location="'POST_{tenant}-duty-assignmen'!A1" display="/{tenant}/duty-assignments/{id}/grade-override" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S31" sqref="S31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1418,17 +1635,20 @@
     <hyperlink ref="A1" location="'Info'!A1" display="&lt;&lt;&lt;&lt;&lt;" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:Q38"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Q33" sqref="Q33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2159,17 +2379,20 @@
     <hyperlink ref="A1" location="'Info'!A1" display="&lt;&lt;&lt;&lt;&lt;" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:Q33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2719,17 +2942,20 @@
     <hyperlink ref="A1" location="'Info'!A1" display="&lt;&lt;&lt;&lt;&lt;" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:Q34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3475,6 +3701,7 @@
     <hyperlink ref="A1" location="'Info'!A1" display="&lt;&lt;&lt;&lt;&lt;" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4010,7 +4237,7 @@
   </sheetPr>
   <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>